<commit_message>
Improved way to make schema updates in tables
</commit_message>
<xml_diff>
--- a/suantrazabilidadapi/utils/data/IntegracionKobo.xlsx
+++ b/suantrazabilidadapi/utils/data/IntegracionKobo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos\Moxietech\Cardano\SUAN\Universidad Cooperativa de Colombia\Plataforma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAA084F-1370-485D-A466-23BCE89AEE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB25836-66F8-459E-928C-0C184FDBA9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078F71B8-FB4B-47FD-968E-8753AE26DA57}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="principalform" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">principalform!$A$1:$F$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">principalform!$A$1:$F$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="97">
   <si>
     <t>I_intro_001</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>A_postulante_email</t>
   </si>
 </sst>
 </file>
@@ -685,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A2FB49-43D1-4E26-AEC3-C094B46DE9AE}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,10 +845,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,7 +865,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -864,7 +876,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -875,20 +887,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" ref="D13:D16" si="1">B13</f>
-        <v>A_vereda</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,14 +898,14 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="1"/>
-        <v>A_municipio</v>
+        <f t="shared" ref="D14:D17" si="1">B14</f>
+        <v>A_vereda</v>
       </c>
       <c r="E14" t="s">
         <v>84</v>
@@ -917,14 +919,14 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>A_matricula</v>
+        <v>A_municipio</v>
       </c>
       <c r="E15" t="s">
         <v>84</v>
@@ -938,14 +940,14 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v>A_ficha_catastral</v>
+        <v>A_matricula</v>
       </c>
       <c r="E16" t="s">
         <v>84</v>
@@ -959,10 +961,20 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>A_ficha_catastral</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,20 +982,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" ref="D18:D20" si="2">B18</f>
-        <v>B_owner</v>
-      </c>
-      <c r="E18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,14 +993,14 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>B_owner_doctype</v>
+        <f t="shared" ref="D19:D21" si="2">B19</f>
+        <v>B_owner</v>
       </c>
       <c r="E19" t="s">
         <v>84</v>
@@ -1012,14 +1014,14 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="2"/>
-        <v>B_owner_id</v>
+        <v>B_owner_doctype</v>
       </c>
       <c r="E20" t="s">
         <v>84</v>
@@ -1032,31 +1034,41 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
+      <c r="B21" t="s">
+        <v>18</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>B_owner_id</v>
       </c>
       <c r="E21" t="s">
         <v>84</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,20 +1076,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" ref="D23:D24" si="3">B23</f>
-        <v>C_ubicacion</v>
-      </c>
-      <c r="E23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1085,17 +1087,17 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="3"/>
-        <v>C_plano_predio</v>
+        <f t="shared" ref="D24:D25" si="3">B24</f>
+        <v>C_ubicacion</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
         <v>88</v>
@@ -1106,10 +1108,20 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="3"/>
+        <v>C_plano_predio</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1117,20 +1129,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
-      </c>
-      <c r="D26" t="str">
-        <f>B26</f>
-        <v>D_area</v>
-      </c>
-      <c r="E26" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,20 +1140,20 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
       <c r="D27" t="str">
         <f>B27</f>
-        <v>D_actual_use</v>
+        <v>D_area</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,13 +1161,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
       <c r="D28" t="str">
-        <f>D27</f>
+        <f>B28</f>
         <v>D_actual_use</v>
       </c>
       <c r="E28" t="s">
@@ -1180,13 +1182,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" ref="D29:D55" si="4">D28</f>
+        <f>D28</f>
         <v>D_actual_use</v>
       </c>
       <c r="E29" t="s">
@@ -1201,13 +1203,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D30:D56" si="4">D29</f>
         <v>D_actual_use</v>
       </c>
       <c r="E30" t="s">
@@ -1222,7 +1224,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -1243,7 +1245,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -1264,7 +1266,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -1285,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -1306,7 +1308,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -1327,7 +1329,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -1348,7 +1350,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -1369,7 +1371,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -1390,7 +1392,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -1411,7 +1413,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -1432,7 +1434,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -1453,7 +1455,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -1474,7 +1476,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -1495,7 +1497,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -1516,7 +1518,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -1537,7 +1539,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -1558,7 +1560,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -1579,7 +1581,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -1600,7 +1602,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -1621,7 +1623,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -1642,7 +1644,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -1663,7 +1665,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -1684,7 +1686,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -1705,7 +1707,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -1726,7 +1728,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -1747,10 +1749,20 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="4"/>
+        <v>D_actual_use</v>
+      </c>
+      <c r="E56" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1758,20 +1770,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
-      </c>
-      <c r="D57" t="str">
-        <f>B57</f>
-        <v>E_restriccion_desc</v>
-      </c>
-      <c r="E57" t="s">
-        <v>86</v>
-      </c>
-      <c r="F57" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1779,14 +1781,14 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
       </c>
       <c r="D58" t="str">
         <f>B58</f>
-        <v>E_resctriccion_other</v>
+        <v>E_restriccion_desc</v>
       </c>
       <c r="E58" t="s">
         <v>86</v>
@@ -1800,10 +1802,20 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
+      </c>
+      <c r="D59" t="str">
+        <f>B59</f>
+        <v>E_resctriccion_other</v>
+      </c>
+      <c r="E59" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1811,20 +1823,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
-      </c>
-      <c r="D60" t="str">
-        <f>B60</f>
-        <v>F_nacimiento_agua</v>
-      </c>
-      <c r="E60" t="s">
-        <v>89</v>
-      </c>
-      <c r="F60" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1832,13 +1834,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
       </c>
       <c r="D61" t="str">
-        <f>D60</f>
+        <f>B61</f>
         <v>F_nacimiento_agua</v>
       </c>
       <c r="E61" t="s">
@@ -1853,13 +1855,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" ref="D62:D69" si="5">D61</f>
+        <f>D61</f>
         <v>F_nacimiento_agua</v>
       </c>
       <c r="E62" t="s">
@@ -1874,13 +1876,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D63:D70" si="5">D62</f>
         <v>F_nacimiento_agua</v>
       </c>
       <c r="E63" t="s">
@@ -1895,7 +1897,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -1916,7 +1918,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -1937,7 +1939,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -1958,7 +1960,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -1979,7 +1981,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -2000,7 +2002,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -2021,10 +2023,20 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="5"/>
+        <v>F_nacimiento_agua</v>
+      </c>
+      <c r="E70" t="s">
+        <v>89</v>
+      </c>
+      <c r="F70" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2032,20 +2044,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
-      </c>
-      <c r="D71" t="str">
-        <f>B71</f>
-        <v>G_habita_predio</v>
-      </c>
-      <c r="E71" t="s">
-        <v>89</v>
-      </c>
-      <c r="F71" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2053,13 +2055,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
       </c>
       <c r="D72" t="str">
-        <f>D71</f>
+        <f>B72</f>
         <v>G_habita_predio</v>
       </c>
       <c r="E72" t="s">
@@ -2074,13 +2076,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" ref="D73:D81" si="6">D72</f>
+        <f>D72</f>
         <v>G_habita_predio</v>
       </c>
       <c r="E73" t="s">
@@ -2095,13 +2097,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D74:D82" si="6">D73</f>
         <v>G_habita_predio</v>
       </c>
       <c r="E74" t="s">
@@ -2116,7 +2118,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -2137,7 +2139,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -2158,7 +2160,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -2179,7 +2181,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -2200,7 +2202,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -2221,7 +2223,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -2242,7 +2244,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -2263,10 +2265,20 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="6"/>
+        <v>G_habita_predio</v>
+      </c>
+      <c r="E82" t="s">
+        <v>89</v>
+      </c>
+      <c r="F82" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2274,20 +2286,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
-      </c>
-      <c r="D83" t="str">
-        <f t="shared" ref="D83:D85" si="7">B83</f>
-        <v>H_asistance_desc</v>
-      </c>
-      <c r="E83" t="s">
-        <v>84</v>
-      </c>
-      <c r="F83" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2295,14 +2297,14 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="7"/>
-        <v>H_aliados_estrategicos_desc</v>
+        <f t="shared" ref="D84:D86" si="7">B84</f>
+        <v>H_asistance_desc</v>
       </c>
       <c r="E84" t="s">
         <v>84</v>
@@ -2316,14 +2318,14 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="7"/>
-        <v>H_grupo_comunitario_desc</v>
+        <v>H_aliados_estrategicos_desc</v>
       </c>
       <c r="E85" t="s">
         <v>84</v>
@@ -2332,8 +2334,29 @@
         <v>88</v>
       </c>
     </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>83</v>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="7"/>
+        <v>H_grupo_comunitario_desc</v>
+      </c>
+      <c r="E86" t="s">
+        <v>84</v>
+      </c>
+      <c r="F86" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F85" xr:uid="{76A2FB49-43D1-4E26-AEC3-C094B46DE9AE}"/>
+  <autoFilter ref="A1:F86" xr:uid="{76A2FB49-43D1-4E26-AEC3-C094B46DE9AE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>